<commit_message>
Meta update before mini expansion
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/RenascentMeta.xlsx
+++ b/Excel_and_CSV/RenascentMeta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D67DEA2-20F9-47C4-B6D8-F350CCA35450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7C5FF8-FB31-40BA-AEE5-D26493C0521F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="224">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -661,9 +661,6 @@
     <t>Sword-Swinging Bandit</t>
   </si>
   <si>
-    <t>76VAc</t>
-  </si>
-  <si>
     <t>Mysteria Machina Rune</t>
   </si>
   <si>
@@ -683,6 +680,18 @@
   </si>
   <si>
     <t>72_IA</t>
+  </si>
+  <si>
+    <t>Aggro Bayleon Sword</t>
+  </si>
+  <si>
+    <t>76mGC</t>
+  </si>
+  <si>
+    <t>72DkI</t>
+  </si>
+  <si>
+    <t>Vagabond Lizard</t>
   </si>
 </sst>
 </file>
@@ -1011,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H994"/>
+  <dimension ref="A1:H995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1278,10 +1287,10 @@
         <v>194</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>12</v>
@@ -1292,7 +1301,7 @@
     </row>
     <row r="11" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>30</v>
@@ -1344,7 +1353,7 @@
     </row>
     <row r="13" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>30</v>
@@ -1356,10 +1365,10 @@
         <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>219</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>220</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>12</v>
@@ -1394,61 +1403,61 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>60</v>
+    <row r="15" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>214</v>
+        <v>56</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>51</v>
@@ -1466,30 +1475,30 @@
         <v>60</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>12</v>
+        <v>67</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>61</v>
+      <c r="A18" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>12</v>
@@ -1500,22 +1509,22 @@
     </row>
     <row r="19" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>67</v>
+      <c r="C19" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>12</v>
@@ -1525,23 +1534,23 @@
       </c>
     </row>
     <row r="20" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>64</v>
+      <c r="A20" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>12</v>
@@ -1550,9 +1559,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>51</v>
@@ -1564,10 +1573,10 @@
         <v>66</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>12</v>
@@ -1578,48 +1587,48 @@
     </row>
     <row r="22" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>12</v>
@@ -1630,22 +1639,22 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>79</v>
+      <c r="C24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>12</v>
@@ -1654,24 +1663,24 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>12</v>
@@ -1682,22 +1691,22 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>12</v>
@@ -1708,22 +1717,22 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>217</v>
+        <v>85</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>218</v>
+        <v>86</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>204</v>
+        <v>87</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>205</v>
+        <v>88</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>12</v>
@@ -1734,74 +1743,74 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="G29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>12</v>
@@ -1811,23 +1820,23 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>105</v>
+      <c r="A31" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>12</v>
@@ -1838,22 +1847,22 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>95</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>12</v>
@@ -1864,100 +1873,100 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="G34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>125</v>
+      <c r="C35" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>127</v>
+        <v>123</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>134</v>
+      <c r="A36" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>133</v>
+      <c r="C36" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>12</v>
@@ -1968,22 +1977,22 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>12</v>
@@ -1993,75 +2002,75 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>129</v>
+      <c r="A38" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E39" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>148</v>
+      <c r="C40" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>12</v>
@@ -2071,55 +2080,55 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>149</v>
+      <c r="A41" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G41" s="12" t="s">
+      <c r="G42" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" s="12" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2133,15 +2142,15 @@
         <v>155</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>155</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="G43" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H43" s="12" t="s">
@@ -2150,42 +2159,42 @@
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>141</v>
       </c>
       <c r="C44" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D45" s="12" t="s">
         <v>160</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="G44" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>153</v>
       </c>
       <c r="E45" s="12" t="s">
         <v>152</v>
@@ -2201,23 +2210,23 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>165</v>
+      <c r="A46" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>153</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>12</v>
@@ -2226,7 +2235,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
         <v>162</v>
       </c>
@@ -2237,7 +2246,7 @@
         <v>164</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>178</v>
@@ -2253,95 +2262,95 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="H50" s="12" t="s">
-        <v>181</v>
+      <c r="G50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="B51" s="13" t="s">
         <v>163</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="E51" s="12" t="s">
         <v>178</v>
@@ -2356,50 +2365,50 @@
         <v>181</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="13" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B52" s="13" t="s">
         <v>163</v>
       </c>
       <c r="C52" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="G52" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="H52" s="12" t="s">
         <v>181</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="B53" s="13" t="s">
         <v>163</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>210</v>
+        <v>181</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="F53" s="12" t="s">
-        <v>210</v>
+        <v>184</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>12</v>
@@ -2410,31 +2419,56 @@
     </row>
     <row r="54" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
       <c r="B54" s="13" t="s">
         <v>163</v>
       </c>
       <c r="C54" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D55" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="E55" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F55" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="G54" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="G55" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3374,6 +3408,7 @@
     <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Last Update for RSC
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/RenascentMeta.xlsx
+++ b/Excel_and_CSV/RenascentMeta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7C5FF8-FB31-40BA-AEE5-D26493C0521F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA052E42-63A2-487D-9732-9CD1ED210B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="235">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -172,526 +172,559 @@
     <t>6_FIo</t>
   </si>
   <si>
+    <t>Rune</t>
+  </si>
+  <si>
+    <t>Mysteria Rune</t>
+  </si>
+  <si>
+    <t>Anne, Mysterian Imperatrix</t>
+  </si>
+  <si>
+    <t>7B48I</t>
+  </si>
+  <si>
+    <t>Grea, Scorching Fury</t>
+  </si>
+  <si>
+    <t>7B1i2</t>
+  </si>
+  <si>
+    <t>Chaos Rune</t>
+  </si>
+  <si>
+    <t>Whims of Chaos</t>
+  </si>
+  <si>
+    <t>7B2Qw</t>
+  </si>
+  <si>
+    <t>Burn Rune</t>
+  </si>
+  <si>
+    <t>Vincent, the Peacekeeper</t>
+  </si>
+  <si>
+    <t>73RsS</t>
+  </si>
+  <si>
+    <t>Tetra, Serene Sapphire</t>
+  </si>
+  <si>
+    <t>7EuHI</t>
+  </si>
+  <si>
+    <t>Vincent Rune</t>
+  </si>
+  <si>
+    <t>Evolution Rune</t>
+  </si>
+  <si>
+    <t>Buff Dragon</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>Drache, Fiery Dragonlord</t>
+  </si>
+  <si>
+    <t>7BSYy</t>
+  </si>
+  <si>
+    <t>Roost Dragon</t>
+  </si>
+  <si>
+    <t>Resplendent Phoenix</t>
+  </si>
+  <si>
+    <t>73nqY</t>
+  </si>
+  <si>
+    <t>Dragon-Devouring Dread</t>
+  </si>
+  <si>
+    <t>73qGo</t>
+  </si>
+  <si>
+    <t>Evolution Dragon</t>
+  </si>
+  <si>
+    <t>Natura Dragon</t>
+  </si>
+  <si>
+    <t>Djeana, the Stouthearted</t>
+  </si>
+  <si>
+    <t>7FEFY</t>
+  </si>
+  <si>
+    <t>Face Dragon</t>
+  </si>
+  <si>
+    <t>Wyrmfire Engineer</t>
+  </si>
+  <si>
+    <t>73iyC</t>
+  </si>
+  <si>
+    <t>Reggie, Peerless Artisan</t>
+  </si>
+  <si>
+    <t>73qGy</t>
+  </si>
+  <si>
+    <t>Whale Dragon</t>
+  </si>
+  <si>
+    <t>Eternal Whale</t>
+  </si>
+  <si>
+    <t>6_zhi</t>
+  </si>
+  <si>
+    <t>Slaughtering Dragonewt</t>
+  </si>
+  <si>
+    <t>6_zhY</t>
+  </si>
+  <si>
+    <t>Machina Shadow</t>
+  </si>
+  <si>
+    <t>Shadow</t>
+  </si>
+  <si>
+    <t>Aenea, Creative Amethyst</t>
+  </si>
+  <si>
+    <t>7Ff6S</t>
+  </si>
+  <si>
+    <t>Nicola, Enduring Steward</t>
+  </si>
+  <si>
+    <t>7Ff6I</t>
+  </si>
+  <si>
+    <t>Aggro Shadow</t>
+  </si>
+  <si>
+    <t>Bone Fanatic</t>
+  </si>
+  <si>
+    <t>745Mi</t>
+  </si>
+  <si>
+    <t>Grudge Teller</t>
+  </si>
+  <si>
+    <t>745MY</t>
+  </si>
+  <si>
+    <t>Nepthys-Vaseraga Shadow</t>
+  </si>
+  <si>
+    <t>Vaseraga, Shadowed Scythe</t>
+  </si>
+  <si>
+    <t>77-O2</t>
+  </si>
+  <si>
+    <t>Nephthys, Goddess of Amenta</t>
+  </si>
+  <si>
+    <t>70OYc</t>
+  </si>
+  <si>
+    <t>OTK Shadow</t>
+  </si>
+  <si>
+    <t>Soul Box</t>
+  </si>
+  <si>
+    <t>70HDs</t>
+  </si>
+  <si>
+    <t>Ceres, Bride of the Night</t>
+  </si>
+  <si>
+    <t>7BqzI</t>
+  </si>
+  <si>
+    <t>Last Words Shadow</t>
+  </si>
+  <si>
+    <t>Wicked Rebirth</t>
+  </si>
+  <si>
+    <t>7BpFw</t>
+  </si>
+  <si>
+    <t>Ominous Tyrant</t>
+  </si>
+  <si>
+    <t>7Bqzc</t>
+  </si>
+  <si>
+    <t>Volteo Blood</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Volteo, Hedonistic Dealer</t>
+  </si>
+  <si>
+    <t>74b5o</t>
+  </si>
+  <si>
+    <t>Mono Blood</t>
+  </si>
+  <si>
+    <t>Mono, Immortal Garnet</t>
+  </si>
+  <si>
+    <t>7G1Wo</t>
+  </si>
+  <si>
+    <t>Rejuvenate the Spark</t>
+  </si>
+  <si>
+    <t>7F_pQ</t>
+  </si>
+  <si>
+    <t>Evolution Blood</t>
+  </si>
+  <si>
+    <t>Aluzard, Timeworn Vampire</t>
+  </si>
+  <si>
+    <t>7CDNy</t>
+  </si>
+  <si>
+    <t>Bloodtroth Epitaph</t>
+  </si>
+  <si>
+    <t>74Z8o</t>
+  </si>
+  <si>
+    <t>Epitaph Blood</t>
+  </si>
+  <si>
+    <t>Wrath Blood</t>
+  </si>
+  <si>
+    <t>Scrappy Werewolf</t>
+  </si>
+  <si>
+    <t>74Tn2</t>
+  </si>
+  <si>
+    <t>Amulet Haven</t>
+  </si>
+  <si>
+    <t>Haven</t>
+  </si>
+  <si>
+    <t>Jatelant, God of Prosperity</t>
+  </si>
+  <si>
+    <t>7CboS</t>
+  </si>
+  <si>
+    <t>Ward Haven</t>
+  </si>
+  <si>
+    <t>Anvelt, Judgment's Cannon</t>
+  </si>
+  <si>
+    <t>74zWS</t>
+  </si>
+  <si>
+    <t>Lunerian Paladin</t>
+  </si>
+  <si>
+    <t>7CWvy</t>
+  </si>
+  <si>
+    <t>Sanctuary Haven</t>
+  </si>
+  <si>
+    <t>Holy Sanctuary</t>
+  </si>
+  <si>
+    <t>74xJg</t>
+  </si>
+  <si>
+    <t>Ra, Radiance Incarnate</t>
+  </si>
+  <si>
+    <t>719Nc</t>
+  </si>
+  <si>
+    <t>Summit Haven</t>
+  </si>
+  <si>
+    <t>Summit Temple</t>
+  </si>
+  <si>
+    <t>78lSg</t>
+  </si>
+  <si>
+    <t>6Qzmg</t>
+  </si>
+  <si>
+    <t>Banish Haven</t>
+  </si>
+  <si>
+    <t>Priest of the Cudgel</t>
+  </si>
+  <si>
+    <t>60E5y</t>
+  </si>
+  <si>
+    <t>Control Ra Haven</t>
+  </si>
+  <si>
+    <t>Machina Portal</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>Belphomet, Ultimate Creator</t>
+  </si>
+  <si>
+    <t>7GoLy</t>
+  </si>
+  <si>
+    <t>gcvky</t>
+  </si>
+  <si>
+    <t>Artifact Portal</t>
+  </si>
+  <si>
+    <t>Artifact Carrier</t>
+  </si>
+  <si>
+    <t>7Cxmi</t>
+  </si>
+  <si>
+    <t>Mobilized Factory</t>
+  </si>
+  <si>
+    <t>797di</t>
+  </si>
+  <si>
+    <t>Rally Portal</t>
+  </si>
+  <si>
+    <t>Fieran, Havensent Wind God</t>
+  </si>
+  <si>
+    <t>6-UTy</t>
+  </si>
+  <si>
+    <t>Stringmaster</t>
+  </si>
+  <si>
+    <t>75EcC</t>
+  </si>
+  <si>
+    <t>Tolerance Portal</t>
+  </si>
+  <si>
+    <t>Absolute Tolerance</t>
+  </si>
+  <si>
+    <t>7C-D6</t>
+  </si>
+  <si>
+    <t>Tien, Treacherous Trigger</t>
+  </si>
+  <si>
+    <t>79A3o</t>
+  </si>
+  <si>
+    <t>Evolution Portal</t>
+  </si>
+  <si>
+    <t>Feower, Double Blade Flash</t>
+  </si>
+  <si>
+    <t>79A3y</t>
+  </si>
+  <si>
+    <t>Aggro Float Portal</t>
+  </si>
+  <si>
+    <t>Capsule Homunculus</t>
+  </si>
+  <si>
+    <t>75H2I</t>
+  </si>
+  <si>
+    <t>Quixotic Adventurer</t>
+  </si>
+  <si>
+    <t>72BIC</t>
+  </si>
+  <si>
+    <t>Resonance Portal</t>
+  </si>
+  <si>
+    <t>7C-Cy</t>
+  </si>
+  <si>
+    <t>Magna Zero</t>
+  </si>
+  <si>
+    <t>Cat Admiral</t>
+  </si>
+  <si>
+    <t>7AfHi</t>
+  </si>
+  <si>
+    <t>Accelerate Forest</t>
+  </si>
+  <si>
+    <t>Fairy Flowering</t>
+  </si>
+  <si>
+    <t>72fJw</t>
+  </si>
+  <si>
+    <t>Walder, Forest Ranger</t>
+  </si>
+  <si>
+    <t>76QHo</t>
+  </si>
+  <si>
+    <t>76Ns0</t>
+  </si>
+  <si>
+    <t>Wind Fairy</t>
+  </si>
+  <si>
+    <t>Touching Thoughts</t>
+  </si>
+  <si>
+    <t>7FA5w</t>
+  </si>
+  <si>
+    <t>Whimsical Mermaid</t>
+  </si>
+  <si>
+    <t>7F9NC</t>
+  </si>
+  <si>
+    <t>Maisha Portal</t>
+  </si>
+  <si>
+    <t>Maisha, Purgation's Vessel</t>
+  </si>
+  <si>
+    <t>7GoLo</t>
+  </si>
+  <si>
+    <t>Aggro Sword</t>
+  </si>
+  <si>
+    <t>Sword-Swinging Bandit</t>
+  </si>
+  <si>
+    <t>Levin OTK Sword</t>
+  </si>
+  <si>
+    <t>Bayleon Sword</t>
+  </si>
+  <si>
+    <t>Naterra's Future</t>
+  </si>
+  <si>
+    <t>7DjKQ</t>
+  </si>
+  <si>
+    <t>Dramatic Retreat</t>
+  </si>
+  <si>
+    <t>72_IA</t>
+  </si>
+  <si>
+    <t>Aggro Bayleon Sword</t>
+  </si>
+  <si>
+    <t>76mGC</t>
+  </si>
+  <si>
+    <t>72DkI</t>
+  </si>
+  <si>
+    <t>Vagabond Lizard</t>
+  </si>
+  <si>
+    <t>Isabelle, Intrepid Mage</t>
+  </si>
+  <si>
+    <t>7EuHc</t>
+  </si>
+  <si>
+    <t>Eris Haven</t>
+  </si>
+  <si>
+    <t>Eris, Atoned Priestess</t>
+  </si>
+  <si>
+    <t>7GPxc</t>
+  </si>
+  <si>
+    <t>Devilish Diva</t>
+  </si>
+  <si>
+    <t>7F_4Y</t>
+  </si>
+  <si>
+    <t>78lDC</t>
+  </si>
+  <si>
+    <t>Smilecure Priest</t>
+  </si>
+  <si>
+    <t>Control Rune</t>
+  </si>
+  <si>
+    <t>Fif, Prodigious Sorcerer</t>
+  </si>
+  <si>
+    <t>77F_I</t>
+  </si>
+  <si>
+    <t>Aggro Rune</t>
+  </si>
+  <si>
+    <t>Maiser, Neighborhood Hero</t>
+  </si>
+  <si>
+    <t>73RsI</t>
+  </si>
+  <si>
+    <t>Rivaylian Bandit</t>
+  </si>
+  <si>
+    <t>72BI2</t>
+  </si>
+  <si>
+    <t>Burial Rite Shadow</t>
+  </si>
+  <si>
+    <t>Conquering Dreadlord</t>
+  </si>
+  <si>
+    <t>70OYS</t>
+  </si>
+  <si>
     <t>Spellboost Rune</t>
-  </si>
-  <si>
-    <t>Rune</t>
-  </si>
-  <si>
-    <t>Ghios, Sparkling Prism</t>
-  </si>
-  <si>
-    <t>7B48S</t>
-  </si>
-  <si>
-    <t>Runie, Resolute Diviner</t>
-  </si>
-  <si>
-    <t>6_djc</t>
-  </si>
-  <si>
-    <t>Mysteria Rune</t>
-  </si>
-  <si>
-    <t>Anne, Mysterian Imperatrix</t>
-  </si>
-  <si>
-    <t>7B48I</t>
-  </si>
-  <si>
-    <t>Grea, Scorching Fury</t>
-  </si>
-  <si>
-    <t>7B1i2</t>
-  </si>
-  <si>
-    <t>Chaos Rune</t>
-  </si>
-  <si>
-    <t>Whims of Chaos</t>
-  </si>
-  <si>
-    <t>7B2Qw</t>
-  </si>
-  <si>
-    <t>Burn Rune</t>
-  </si>
-  <si>
-    <t>Vincent, the Peacekeeper</t>
-  </si>
-  <si>
-    <t>73RsS</t>
-  </si>
-  <si>
-    <t>Tetra, Serene Sapphire</t>
-  </si>
-  <si>
-    <t>7EuHI</t>
-  </si>
-  <si>
-    <t>Vincent Rune</t>
-  </si>
-  <si>
-    <t>Evolution Rune</t>
-  </si>
-  <si>
-    <t>Buff Dragon</t>
-  </si>
-  <si>
-    <t>Dragon</t>
-  </si>
-  <si>
-    <t>Drache, Fiery Dragonlord</t>
-  </si>
-  <si>
-    <t>7BSYy</t>
-  </si>
-  <si>
-    <t>Roost Dragon</t>
-  </si>
-  <si>
-    <t>Resplendent Phoenix</t>
-  </si>
-  <si>
-    <t>73nqY</t>
-  </si>
-  <si>
-    <t>Dragon-Devouring Dread</t>
-  </si>
-  <si>
-    <t>73qGo</t>
-  </si>
-  <si>
-    <t>Evolution Dragon</t>
-  </si>
-  <si>
-    <t>Natura Dragon</t>
-  </si>
-  <si>
-    <t>Djeana, the Stouthearted</t>
-  </si>
-  <si>
-    <t>7FEFY</t>
-  </si>
-  <si>
-    <t>Face Dragon</t>
-  </si>
-  <si>
-    <t>Wyrmfire Engineer</t>
-  </si>
-  <si>
-    <t>73iyC</t>
-  </si>
-  <si>
-    <t>Reggie, Peerless Artisan</t>
-  </si>
-  <si>
-    <t>73qGy</t>
-  </si>
-  <si>
-    <t>Whale Dragon</t>
-  </si>
-  <si>
-    <t>Eternal Whale</t>
-  </si>
-  <si>
-    <t>6_zhi</t>
-  </si>
-  <si>
-    <t>Slaughtering Dragonewt</t>
-  </si>
-  <si>
-    <t>6_zhY</t>
-  </si>
-  <si>
-    <t>Machina Shadow</t>
-  </si>
-  <si>
-    <t>Shadow</t>
-  </si>
-  <si>
-    <t>Aenea, Creative Amethyst</t>
-  </si>
-  <si>
-    <t>7Ff6S</t>
-  </si>
-  <si>
-    <t>Nicola, Enduring Steward</t>
-  </si>
-  <si>
-    <t>7Ff6I</t>
-  </si>
-  <si>
-    <t>Aggro Shadow</t>
-  </si>
-  <si>
-    <t>Bone Fanatic</t>
-  </si>
-  <si>
-    <t>745Mi</t>
-  </si>
-  <si>
-    <t>Grudge Teller</t>
-  </si>
-  <si>
-    <t>745MY</t>
-  </si>
-  <si>
-    <t>Nepthys-Vaseraga Shadow</t>
-  </si>
-  <si>
-    <t>Vaseraga, Shadowed Scythe</t>
-  </si>
-  <si>
-    <t>77-O2</t>
-  </si>
-  <si>
-    <t>Nephthys, Goddess of Amenta</t>
-  </si>
-  <si>
-    <t>70OYc</t>
-  </si>
-  <si>
-    <t>OTK Shadow</t>
-  </si>
-  <si>
-    <t>Soul Box</t>
-  </si>
-  <si>
-    <t>70HDs</t>
-  </si>
-  <si>
-    <t>Ceres, Bride of the Night</t>
-  </si>
-  <si>
-    <t>7BqzI</t>
-  </si>
-  <si>
-    <t>Last Words Shadow</t>
-  </si>
-  <si>
-    <t>Wicked Rebirth</t>
-  </si>
-  <si>
-    <t>7BpFw</t>
-  </si>
-  <si>
-    <t>Ominous Tyrant</t>
-  </si>
-  <si>
-    <t>7Bqzc</t>
-  </si>
-  <si>
-    <t>Volteo Blood</t>
-  </si>
-  <si>
-    <t>Blood</t>
-  </si>
-  <si>
-    <t>Volteo, Hedonistic Dealer</t>
-  </si>
-  <si>
-    <t>74b5o</t>
-  </si>
-  <si>
-    <t>Mono Blood</t>
-  </si>
-  <si>
-    <t>Mono, Immortal Garnet</t>
-  </si>
-  <si>
-    <t>7G1Wo</t>
-  </si>
-  <si>
-    <t>Rejuvenate the Spark</t>
-  </si>
-  <si>
-    <t>7F_pQ</t>
-  </si>
-  <si>
-    <t>Evolution Blood</t>
-  </si>
-  <si>
-    <t>Aluzard, Timeworn Vampire</t>
-  </si>
-  <si>
-    <t>7CDNy</t>
-  </si>
-  <si>
-    <t>Bloodtroth Epitaph</t>
-  </si>
-  <si>
-    <t>74Z8o</t>
-  </si>
-  <si>
-    <t>Epitaph Blood</t>
-  </si>
-  <si>
-    <t>Wrath Blood</t>
-  </si>
-  <si>
-    <t>Scrappy Werewolf</t>
-  </si>
-  <si>
-    <t>74Tn2</t>
-  </si>
-  <si>
-    <t>Darhold, Abyssal Contract</t>
-  </si>
-  <si>
-    <t>70myy</t>
-  </si>
-  <si>
-    <t>Amulet Haven</t>
-  </si>
-  <si>
-    <t>Haven</t>
-  </si>
-  <si>
-    <t>Jatelant, God of Prosperity</t>
-  </si>
-  <si>
-    <t>7CboS</t>
-  </si>
-  <si>
-    <t>Ward Haven</t>
-  </si>
-  <si>
-    <t>Anvelt, Judgment's Cannon</t>
-  </si>
-  <si>
-    <t>74zWS</t>
-  </si>
-  <si>
-    <t>Lunerian Paladin</t>
-  </si>
-  <si>
-    <t>7CWvy</t>
-  </si>
-  <si>
-    <t>Sanctuary Haven</t>
-  </si>
-  <si>
-    <t>Holy Sanctuary</t>
-  </si>
-  <si>
-    <t>74xJg</t>
-  </si>
-  <si>
-    <t>Ra, Radiance Incarnate</t>
-  </si>
-  <si>
-    <t>719Nc</t>
-  </si>
-  <si>
-    <t>Summit Haven</t>
-  </si>
-  <si>
-    <t>Summit Temple</t>
-  </si>
-  <si>
-    <t>78lSg</t>
-  </si>
-  <si>
-    <t>6Qzmg</t>
-  </si>
-  <si>
-    <t>Banish Haven</t>
-  </si>
-  <si>
-    <t>Priest of the Cudgel</t>
-  </si>
-  <si>
-    <t>60E5y</t>
-  </si>
-  <si>
-    <t>Control Ra Haven</t>
-  </si>
-  <si>
-    <t>Machina Portal</t>
-  </si>
-  <si>
-    <t>Portal</t>
-  </si>
-  <si>
-    <t>Belphomet, Ultimate Creator</t>
-  </si>
-  <si>
-    <t>7GoLy</t>
-  </si>
-  <si>
-    <t>gcvky</t>
-  </si>
-  <si>
-    <t>Artifact Portal</t>
-  </si>
-  <si>
-    <t>Artifact Carrier</t>
-  </si>
-  <si>
-    <t>7Cxmi</t>
-  </si>
-  <si>
-    <t>Mobilized Factory</t>
-  </si>
-  <si>
-    <t>797di</t>
-  </si>
-  <si>
-    <t>Rally Portal</t>
-  </si>
-  <si>
-    <t>Fieran, Havensent Wind God</t>
-  </si>
-  <si>
-    <t>6-UTy</t>
-  </si>
-  <si>
-    <t>Stringmaster</t>
-  </si>
-  <si>
-    <t>75EcC</t>
-  </si>
-  <si>
-    <t>Tolerance Portal</t>
-  </si>
-  <si>
-    <t>Absolute Tolerance</t>
-  </si>
-  <si>
-    <t>7C-D6</t>
-  </si>
-  <si>
-    <t>Tien, Treacherous Trigger</t>
-  </si>
-  <si>
-    <t>79A3o</t>
-  </si>
-  <si>
-    <t>Evolution Portal</t>
-  </si>
-  <si>
-    <t>Feower, Double Blade Flash</t>
-  </si>
-  <si>
-    <t>79A3y</t>
-  </si>
-  <si>
-    <t>Aggro Float Portal</t>
-  </si>
-  <si>
-    <t>Capsule Homunculus</t>
-  </si>
-  <si>
-    <t>75H2I</t>
-  </si>
-  <si>
-    <t>Quixotic Adventurer</t>
-  </si>
-  <si>
-    <t>72BIC</t>
-  </si>
-  <si>
-    <t>Resonance Portal</t>
-  </si>
-  <si>
-    <t>7C-Cy</t>
-  </si>
-  <si>
-    <t>Magna Zero</t>
-  </si>
-  <si>
-    <t>Cat Admiral</t>
-  </si>
-  <si>
-    <t>7AfHi</t>
-  </si>
-  <si>
-    <t>Marie, Flowery Magician</t>
-  </si>
-  <si>
-    <t>7EpOo</t>
-  </si>
-  <si>
-    <t>Accelerate Forest</t>
-  </si>
-  <si>
-    <t>Fairy Flowering</t>
-  </si>
-  <si>
-    <t>72fJw</t>
-  </si>
-  <si>
-    <t>Walder, Forest Ranger</t>
-  </si>
-  <si>
-    <t>76QHo</t>
-  </si>
-  <si>
-    <t>76Ns0</t>
-  </si>
-  <si>
-    <t>Wind Fairy</t>
-  </si>
-  <si>
-    <t>Touching Thoughts</t>
-  </si>
-  <si>
-    <t>7FA5w</t>
-  </si>
-  <si>
-    <t>Whimsical Mermaid</t>
-  </si>
-  <si>
-    <t>7F9NC</t>
-  </si>
-  <si>
-    <t>Maisha Portal</t>
-  </si>
-  <si>
-    <t>Maisha, Purgation's Vessel</t>
-  </si>
-  <si>
-    <t>7GoLo</t>
-  </si>
-  <si>
-    <t>Aggro Sword</t>
-  </si>
-  <si>
-    <t>Sword-Swinging Bandit</t>
-  </si>
-  <si>
-    <t>Mysteria Machina Rune</t>
-  </si>
-  <si>
-    <t>Levin OTK Sword</t>
-  </si>
-  <si>
-    <t>Bayleon Sword</t>
-  </si>
-  <si>
-    <t>Naterra's Future</t>
-  </si>
-  <si>
-    <t>7DjKQ</t>
-  </si>
-  <si>
-    <t>Dramatic Retreat</t>
-  </si>
-  <si>
-    <t>72_IA</t>
-  </si>
-  <si>
-    <t>Aggro Bayleon Sword</t>
-  </si>
-  <si>
-    <t>76mGC</t>
-  </si>
-  <si>
-    <t>72DkI</t>
-  </si>
-  <si>
-    <t>Vagabond Lizard</t>
   </si>
 </sst>
 </file>
@@ -1020,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H995"/>
+  <dimension ref="A1:H997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1093,22 +1126,22 @@
     </row>
     <row r="3" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>12</v>
@@ -1157,10 +1190,10 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>12</v>
@@ -1255,10 +1288,10 @@
         <v>30</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>34</v>
@@ -1275,22 +1308,22 @@
     </row>
     <row r="10" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>12</v>
@@ -1301,7 +1334,7 @@
     </row>
     <row r="11" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>30</v>
@@ -1353,7 +1386,7 @@
     </row>
     <row r="13" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>30</v>
@@ -1365,10 +1398,10 @@
         <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>12</v>
@@ -1405,7 +1438,7 @@
     </row>
     <row r="15" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>30</v>
@@ -1417,10 +1450,10 @@
         <v>35</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>12</v>
@@ -1431,10 +1464,10 @@
     </row>
     <row r="16" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>52</v>
@@ -1448,19 +1481,19 @@
       <c r="F16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>59</v>
+      <c r="G16" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>57</v>
@@ -1469,88 +1502,88 @@
         <v>58</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="B20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>12</v>
@@ -1561,100 +1594,100 @@
     </row>
     <row r="21" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>12</v>
@@ -1665,22 +1698,22 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>12</v>
@@ -1691,10 +1724,10 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>19</v>
@@ -1703,10 +1736,10 @@
         <v>20</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>12</v>
@@ -1717,22 +1750,22 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>12</v>
@@ -1743,22 +1776,22 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>12</v>
@@ -1769,22 +1802,22 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>12</v>
@@ -1795,22 +1828,22 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>12</v>
@@ -1821,22 +1854,22 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>12</v>
@@ -1847,22 +1880,22 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>12</v>
@@ -1873,49 +1906,49 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E34" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="G34" s="2" t="s">
         <v>12</v>
       </c>
@@ -1923,76 +1956,76 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>120</v>
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>133</v>
+      <c r="E37" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>12</v>
@@ -2003,180 +2036,180 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E41" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="B42" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="D42" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="E42" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="F42" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="G42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="B43" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" s="12" t="s">
+      <c r="E43" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="B44" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="D44" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>157</v>
-      </c>
       <c r="E44" s="13" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="G44" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H44" s="12" t="s">
@@ -2185,22 +2218,22 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>12</v>
@@ -2210,23 +2243,23 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="C46" s="12" t="s">
+      <c r="A46" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="13" t="s">
         <v>152</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>153</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>12</v>
@@ -2236,231 +2269,231 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="E51" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="F51" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="G51" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E47" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="G47" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H47" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D48" s="8" t="s">
+      <c r="B52" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E48" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="G48" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H48" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="D52" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C49" s="3" t="s">
+      <c r="E52" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="F52" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="G52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="B54" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="D54" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="E54" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G54" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="H54" s="12" t="s">
         <v>174</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="H51" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="H52" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="F54" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="E55" s="13" t="s">
-        <v>188</v>
+        <v>174</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>176</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>12</v>
@@ -2469,8 +2502,58 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3409,6 +3492,8 @@
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>